<commit_message>
Finish Provat PM point density extraction
</commit_message>
<xml_diff>
--- a/arcgis_zonal_fmps_and_allcity200_zonal /provat PointDe_PM extraction 033019/buffer_justPointDePM.xlsx
+++ b/arcgis_zonal_fmps_and_allcity200_zonal /provat PointDe_PM extraction 033019/buffer_justPointDePM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugh/Box Sync/from_dropbox/ACE hugh/ACE R/provat_ufp_lur/provat PointDe_PM extraction 033019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugh/Box Sync/from_dropbox/ACE hugh/ACE R/provat_ufp_lur/arcgis_zonal_fmps_and_allcity200_zonal /provat PointDe_PM extraction 033019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A0564B-3C93-644D-BF69-E1523ECD1975}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD8E5D6-E355-654D-B77C-034FB4DE9411}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -954,13 +954,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="89" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>